<commit_message>
Background object scrolling update
update
</commit_message>
<xml_diff>
--- a/Assets/Resources/XML/Database.xlsx
+++ b/Assets/Resources/XML/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12870" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Item Data" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,505 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>이현중</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이현중</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Number : 0~5
+ReturnTown : </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>마을로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>복귀
+RepeatThisFloor : 이번층 반복</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FreePassNextFloor : </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>다음</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>층</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">스킵
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">FreePassThisFloor : </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>사용시</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이번</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>층</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">스킵
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SetBossFloor : </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>다음</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>층</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>보스</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>소환</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이현중</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Health : </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>체력을</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>회복한다</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">.
+Bullet : </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>탄을</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>보충한다</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">.
+Attack : </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>공격력을</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>증가시킨다</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">.
+Defense : </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>방어력을</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>증가시킨다</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,7 +545,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="118">
   <si>
     <t>itemName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,431 +595,425 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RepeatThisFloor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매직</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReturnPreFloor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유니크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FreePassNextFloor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유니크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FreePassThisFloor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격속도를 증가시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack Speed UP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어력을 증가시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defense UP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unlock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력을 증가시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack UP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력을 회복한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Passive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillTimeDuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillOnCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillDescription</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillRarity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterMoveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterAttackSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterAttackRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterPopChance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterDefense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goblin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goblin Acher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ogre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wolf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokkaebi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음층에 보스를 소환하는 탑의 조각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이번층을 넘어가는 탑의 조각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음층을 넘어가는 탑의 조각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자가 적힌 탑의 조각</t>
+  </si>
+  <si>
+    <t>반복하는 탑의 조각</t>
+  </si>
+  <si>
+    <t>화살표가 그려진 탑의 조각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ReturnTown</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RepeatThisFloor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>숫자가 적힌 돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>숫자가 적힌 돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>숫자가 적힌 돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마을로 돌아가는 돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>반복하는 돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>health</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>moveSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>defense</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매직</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>왼쪽 화살표가 그려진 돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReturnPreFloor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bullet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유니크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다음층을 넘어가는 돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FreePassNextFloor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>health</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유니크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이번층을 넘어가는 돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FreePassThisFloor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bullet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격속도를 증가시킨다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack Speed UP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Active</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방어력을 증가시킨다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Defense UP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unlock</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격력을 증가시킨다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack UP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>체력을 회복한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Passive</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillTimeDuration</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillOnCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillDescription</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillRarity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterMoveSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterAttackSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterAttackRange</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterPopChance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monsterDefense</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Frog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Goblin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Goblin Acher</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ogre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wolf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>70</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bear</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokkaebi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>150</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5</t>
+    <t>Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bullet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bullet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마을로 돌아갈 수 있는 탑의 조각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -531,7 +1024,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +1039,34 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1074,11 +1595,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1127,13 +1648,13 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="G2" s="2">
         <v>20</v>
@@ -1150,16 +1671,16 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>117</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1173,13 +1694,13 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1187,7 +1708,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1196,13 +1717,13 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -1219,13 +1740,13 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -1242,13 +1763,13 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -1265,13 +1786,13 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -1288,13 +1809,13 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1302,7 +1823,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1311,13 +1832,13 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="G10">
         <v>50</v>
@@ -1325,7 +1846,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1334,15 +1855,38 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12">
         <v>10</v>
       </c>
     </row>
@@ -1350,8 +1894,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1378,36 +1923,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
@@ -1416,7 +1961,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1">
         <v>5</v>
@@ -1425,15 +1970,15 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1">
         <v>101</v>
@@ -1442,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1">
         <v>5</v>
@@ -1451,15 +1996,15 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1">
         <v>102</v>
@@ -1468,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1">
         <v>5</v>
@@ -1479,10 +2024,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1">
         <v>103</v>
@@ -1491,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1">
         <v>5</v>
@@ -1514,7 +2059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -1533,60 +2078,60 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1594,28 +2139,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1623,28 +2168,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1652,28 +2197,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1681,28 +2226,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1710,28 +2255,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1739,57 +2284,57 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
player attack xml update
update
</commit_message>
<xml_diff>
--- a/Assets/Resources/XML/Database.xlsx
+++ b/Assets/Resources/XML/Database.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12870" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Item Data" sheetId="1" r:id="rId1"/>
     <sheet name="Skill Data" sheetId="3" r:id="rId2"/>
     <sheet name="Monster Data" sheetId="4" r:id="rId3"/>
+    <sheet name="Player Attack Data" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -538,14 +539,26 @@
   <connection id="4" name="MonsterDataBaseBasic1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\MonsterDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="5" name="SkillDataBaseBasic" type="4" refreshedVersion="0" background="1">
+  <connection id="5" name="MonsterDataBaseBasic2" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\MonsterDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="6" name="PlayerAttackBasic" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\PlayerAttackBasic.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="7" name="PlayerAttackBasic1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\PlayerAttackBasic.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="8" name="PlayerAttackBasic2" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\PlayerAttackBasic.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="9" name="SkillDataBaseBasic" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\SkillDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="173">
   <si>
     <t>itemName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1078,6 +1091,146 @@
   </si>
   <si>
     <t>보스를 소환하는 보석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterWeight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackXPoint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackYPoint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackXRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackYRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>knockBack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>distanceMultiply</t>
+  </si>
+  <si>
+    <t>attackMultiply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear_X_Attack</t>
+  </si>
+  <si>
+    <t>spear_XX_Attack</t>
+  </si>
+  <si>
+    <t>spear_XXX_Attack</t>
+  </si>
+  <si>
+    <t>spear_XFX_Attack</t>
+  </si>
+  <si>
+    <t>spear_XFXFX_Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear_JumpX_Attack</t>
+  </si>
+  <si>
+    <t>spear_Y_Attack</t>
+  </si>
+  <si>
+    <t>spear_YUp_Attack</t>
+  </si>
+  <si>
+    <t>gun_X_Attack</t>
+  </si>
+  <si>
+    <t>gun_XX_Attack</t>
+  </si>
+  <si>
+    <t>gun_XXX_Attack</t>
+  </si>
+  <si>
+    <t>gun_XFX_Attack</t>
+  </si>
+  <si>
+    <t>gun_XFXFX_Attack</t>
+  </si>
+  <si>
+    <t>gun_JumpX_Attack</t>
+  </si>
+  <si>
+    <t>gun_Y_Attack</t>
+  </si>
+  <si>
+    <t>gun_YUp_Attack</t>
+  </si>
+  <si>
+    <t>0.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1321,7 +1474,10 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1409,7 +1565,7 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema6">
+  <Schema ID="Schema4">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="MonsterDataBase">
         <xsd:complexType>
@@ -1425,6 +1581,29 @@
                 <xsd:attribute name="monsterAttack" form="unqualified" type="xsd:string"/>
                 <xsd:attribute name="monsterDefense" form="unqualified" type="xsd:string"/>
                 <xsd:attribute name="monsterPopChance" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="monsterWeight" form="unqualified" type="xsd:string"/>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema7">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="PlayerAttackDataBase">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Field" form="unqualified">
+              <xsd:complexType>
+                <xsd:attribute name="attackType" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="attackXPoint" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="attackYPoint" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="attackXRange" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="attackYRange" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="attackMultiply" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="distanceMultiply" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="knockBack" form="unqualified" type="xsd:string"/>
               </xsd:complexType>
             </xsd:element>
           </xsd:sequence>
@@ -1435,11 +1614,14 @@
   <Map ID="2" Name="ItemDataBase_맵" RootElement="ItemDataBase" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="6" Name="MonsterDataBase_맵" RootElement="MonsterDataBase" SchemaID="Schema6" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="4" DataBindingLoadMode="1"/>
+  <Map ID="8" Name="MonsterDataBase_맵" RootElement="MonsterDataBase" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="5" DataBindingLoadMode="1"/>
+  </Map>
+  <Map ID="12" Name="PlayerAttackDataBase_맵" RootElement="PlayerAttackDataBase" SchemaID="Schema7" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="8" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="3" Name="SkillDataBase_맵" RootElement="SkillDataBase" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="5" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="9" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
@@ -1478,7 +1660,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A1:G5" tableType="xml" totalsRowShown="0" connectionId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A1:G5" tableType="xml" totalsRowShown="0" connectionId="9">
   <autoFilter ref="A1:G5"/>
   <tableColumns count="7">
     <tableColumn id="1" uniqueName="skillType" name="skillType">
@@ -1490,7 +1672,7 @@
     <tableColumn id="3" uniqueName="skillCode" name="skillCode">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillCode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="skillRarity" name="skillRarity" dataDxfId="9">
+    <tableColumn id="4" uniqueName="skillRarity" name="skillRarity" dataDxfId="10">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillRarity" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="skillDescription" name="skillDescription">
@@ -1508,35 +1690,71 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="표4" displayName="표4" ref="A1:I11" tableType="xml" totalsRowShown="0" connectionId="4">
-  <autoFilter ref="A1:I11"/>
-  <tableColumns count="9">
-    <tableColumn id="1" uniqueName="monsterCode" name="monsterCode" dataDxfId="8">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterCode" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="표4" displayName="표4" ref="A1:J11" tableType="xml" totalsRowShown="0" connectionId="5">
+  <autoFilter ref="A1:J11"/>
+  <tableColumns count="10">
+    <tableColumn id="1" uniqueName="monsterCode" name="monsterCode" dataDxfId="9">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterCode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="monsterName" name="monsterName" dataDxfId="7">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterName" xmlDataType="string"/>
+    <tableColumn id="2" uniqueName="monsterName" name="monsterName" dataDxfId="8">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterName" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="monsterHP" name="monsterHP" dataDxfId="6">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterHP" xmlDataType="string"/>
+    <tableColumn id="3" uniqueName="monsterHP" name="monsterHP" dataDxfId="7">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterHP" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="monsterMoveSpeed" name="monsterMoveSpeed" dataDxfId="5">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterMoveSpeed" xmlDataType="string"/>
+    <tableColumn id="4" uniqueName="monsterMoveSpeed" name="monsterMoveSpeed" dataDxfId="6">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterMoveSpeed" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="monsterAttackSpeed" name="monsterAttackSpeed" dataDxfId="4">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterAttackSpeed" xmlDataType="string"/>
+    <tableColumn id="5" uniqueName="monsterAttackSpeed" name="monsterAttackSpeed" dataDxfId="5">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterAttackSpeed" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="monsterAttackRange" name="monsterAttackRange" dataDxfId="3">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterAttackRange" xmlDataType="string"/>
+    <tableColumn id="6" uniqueName="monsterAttackRange" name="monsterAttackRange" dataDxfId="4">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterAttackRange" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="monsterAttack" name="monsterAttack" dataDxfId="2">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterAttack" xmlDataType="string"/>
+    <tableColumn id="7" uniqueName="monsterAttack" name="monsterAttack" dataDxfId="3">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterAttack" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="monsterDefense" name="monsterDefense" dataDxfId="1">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterDefense" xmlDataType="string"/>
+    <tableColumn id="8" uniqueName="monsterDefense" name="monsterDefense" dataDxfId="2">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterDefense" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="monsterPopChance" name="monsterPopChance" dataDxfId="0">
-      <xmlColumnPr mapId="6" xpath="/MonsterDataBase/Field/@monsterPopChance" xmlDataType="string"/>
+    <tableColumn id="9" uniqueName="monsterPopChance" name="monsterPopChance" dataDxfId="1">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterPopChance" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="10" uniqueName="monsterWeight" name="monsterWeight" dataDxfId="0">
+      <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterWeight" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="표3" displayName="표3" ref="A1:H17" tableType="xml" totalsRowShown="0" connectionId="8">
+  <autoFilter ref="A1:H17"/>
+  <tableColumns count="8">
+    <tableColumn id="1" uniqueName="attackType" name="attackType">
+      <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackType" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="attackXPoint" name="attackXPoint">
+      <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackXPoint" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" uniqueName="attackYPoint" name="attackYPoint">
+      <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackYPoint" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" uniqueName="attackXRange" name="attackXRange">
+      <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackXRange" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="5" uniqueName="attackYRange" name="attackYRange">
+      <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackYRange" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" uniqueName="attackMultiply" name="attackMultiply">
+      <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackMultiply" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="7" uniqueName="distanceMultiply" name="distanceMultiply">
+      <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@distanceMultiply" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="8" uniqueName="knockBack" name="knockBack">
+      <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@knockBack" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1808,7 +2026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -2730,26 +2948,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="21.125" customWidth="1"/>
+    <col min="6" max="6" width="21.875" customWidth="1"/>
     <col min="7" max="7" width="17.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.625" customWidth="1"/>
     <col min="9" max="9" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2777,8 +2996,11 @@
       <c r="I1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -2806,8 +3028,11 @@
       <c r="I2" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2835,8 +3060,11 @@
       <c r="I3" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2864,8 +3092,11 @@
       <c r="I4" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2893,8 +3124,11 @@
       <c r="I5" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2922,8 +3156,11 @@
       <c r="I6" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2951,8 +3188,11 @@
       <c r="I7" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2980,8 +3220,11 @@
       <c r="I8" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -3009,8 +3252,11 @@
       <c r="I9" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1001</v>
       </c>
@@ -3038,8 +3284,11 @@
       <c r="I10" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1002</v>
       </c>
@@ -3066,6 +3315,481 @@
       </c>
       <c r="I11" s="1" t="s">
         <v>117</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3">
+        <v>0.8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.8</v>
+      </c>
+      <c r="F3">
+        <v>1.2</v>
+      </c>
+      <c r="G3">
+        <v>1.25</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4">
+        <v>0.8</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1.5</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5">
+        <v>0.8</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1.2</v>
+      </c>
+      <c r="G5">
+        <v>1.25</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1.2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1.5</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>-0.6</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1.2</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9">
+        <v>0.8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1.5</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10">
+        <v>1.2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1.2</v>
+      </c>
+      <c r="E10">
+        <v>1.2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11">
+        <v>1.2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1.2</v>
+      </c>
+      <c r="E11">
+        <v>1.2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12">
+        <v>1.2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1.2</v>
+      </c>
+      <c r="E12">
+        <v>1.2</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>-1.25</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13">
+        <v>1.2</v>
+      </c>
+      <c r="C13">
+        <v>-0.1</v>
+      </c>
+      <c r="D13">
+        <v>1.2</v>
+      </c>
+      <c r="E13">
+        <v>0.8</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>1.25</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14">
+        <v>1.2</v>
+      </c>
+      <c r="C14">
+        <v>-0.6</v>
+      </c>
+      <c r="D14">
+        <v>1.2</v>
+      </c>
+      <c r="E14">
+        <v>1.2</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15">
+        <v>1.2</v>
+      </c>
+      <c r="C15">
+        <v>-0.6</v>
+      </c>
+      <c r="D15">
+        <v>1.2</v>
+      </c>
+      <c r="E15">
+        <v>1.2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update db playercharacter atk data
</commit_message>
<xml_diff>
--- a/Assets/Resources/XML/Database.xlsx
+++ b/Assets/Resources/XML/Database.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Chrono Knights\Chrono_Knights\Assets\Resources\XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87081F3A-FA89-4D20-A8D2-03248C7BDE6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12870" activeTab="3"/>
+    <workbookView xWindow="1110" yWindow="1155" windowWidth="22110" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item Data" sheetId="1" r:id="rId1"/>
@@ -27,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>이현중</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -310,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -526,39 +527,39 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="ItemDataBase" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="ItemDataBase" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\xml\ItemDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" name="ItemDataBaseBasic" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="ItemDataBaseBasic" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\xml\ItemDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" name="MonsterDataBaseBasic" type="4" refreshedVersion="0" background="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="MonsterDataBaseBasic" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\MonsterDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="4" name="MonsterDataBaseBasic1" type="4" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="MonsterDataBaseBasic1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\MonsterDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="5" name="MonsterDataBaseBasic2" type="4" refreshedVersion="0" background="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="MonsterDataBaseBasic2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\MonsterDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="6" name="PlayerAttackBasic" type="4" refreshedVersion="0" background="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="PlayerAttackBasic" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\PlayerAttackBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="7" name="PlayerAttackBasic1" type="4" refreshedVersion="0" background="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="PlayerAttackBasic1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\PlayerAttackBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="8" name="PlayerAttackBasic2" type="4" refreshedVersion="0" background="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="PlayerAttackBasic2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\PlayerAttackBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="9" name="SkillDataBaseBasic" type="4" refreshedVersion="0" background="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="SkillDataBaseBasic" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\sources\unity\True_Project_B\Chrono_Knights\Assets\Resources\XML\SkillDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="178">
   <si>
     <t>itemName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1181,9 +1182,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>spear_JumpX_Attack</t>
-  </si>
-  <si>
     <t>spear_Y_Attack</t>
   </si>
   <si>
@@ -1231,13 +1229,37 @@
   </si>
   <si>
     <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear_Jump_X_Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear_Jump_XX_Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear_Jump_XXX_Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear_Jump_Y_Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear_Jump_Down_X_Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear_Jump_Up_X_Attack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
@@ -1627,31 +1649,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="표2" displayName="표2" ref="A1:G31" tableType="xml" totalsRowShown="0" connectionId="2">
-  <autoFilter ref="A1:G31"/>
-  <sortState ref="A2:G31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표2" displayName="표2" ref="A1:G31" tableType="xml" totalsRowShown="0" connectionId="2">
+  <autoFilter ref="A1:G31" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
     <sortCondition ref="C1:C31"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" uniqueName="itemName" name="itemName">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="itemName" name="itemName">
       <xmlColumnPr mapId="2" xpath="/ItemDataBase/Field/@itemName" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="itemRarity" name="itemRarity">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="itemRarity" name="itemRarity">
       <xmlColumnPr mapId="2" xpath="/ItemDataBase/Field/@itemRarity" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="itemCode" name="itemCode">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="itemCode" name="itemCode">
       <xmlColumnPr mapId="2" xpath="/ItemDataBase/Field/@itemCode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="itemDescription" name="itemDescription">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="itemDescription" name="itemDescription">
       <xmlColumnPr mapId="2" xpath="/ItemDataBase/Field/@itemDescription" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="itemType" name="itemType">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="itemType" name="itemType">
       <xmlColumnPr mapId="2" xpath="/ItemDataBase/Field/@itemType" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="itemUsingType" name="itemUsingType">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="itemUsingType" name="itemUsingType">
       <xmlColumnPr mapId="2" xpath="/ItemDataBase/Field/@itemUsingType" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="itemValue" name="itemValue">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="itemValue" name="itemValue">
       <xmlColumnPr mapId="2" xpath="/ItemDataBase/Field/@itemValue" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -1660,28 +1682,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A1:G5" tableType="xml" totalsRowShown="0" connectionId="9">
-  <autoFilter ref="A1:G5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="표1" displayName="표1" ref="A1:G5" tableType="xml" totalsRowShown="0" connectionId="9">
+  <autoFilter ref="A1:G5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" uniqueName="skillType" name="skillType">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" uniqueName="skillType" name="skillType">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillType" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="skillName" name="skillName">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" uniqueName="skillName" name="skillName">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillName" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="skillCode" name="skillCode">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" uniqueName="skillCode" name="skillCode">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillCode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="skillRarity" name="skillRarity" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" uniqueName="skillRarity" name="skillRarity" dataDxfId="10">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillRarity" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="skillDescription" name="skillDescription">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" uniqueName="skillDescription" name="skillDescription">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillDescription" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="skillOnCount" name="skillOnCount">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" uniqueName="skillOnCount" name="skillOnCount">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillOnCount" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="skillTimeDuration" name="skillTimeDuration">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" uniqueName="skillTimeDuration" name="skillTimeDuration">
       <xmlColumnPr mapId="3" xpath="/SkillDataBase/Field/@skillTimeDuration" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -1690,37 +1712,37 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="표4" displayName="표4" ref="A1:J11" tableType="xml" totalsRowShown="0" connectionId="5">
-  <autoFilter ref="A1:J11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="표4" displayName="표4" ref="A1:J11" tableType="xml" totalsRowShown="0" connectionId="5">
+  <autoFilter ref="A1:J11" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" uniqueName="monsterCode" name="monsterCode" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" uniqueName="monsterCode" name="monsterCode" dataDxfId="9">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterCode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="monsterName" name="monsterName" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" uniqueName="monsterName" name="monsterName" dataDxfId="8">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterName" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="monsterHP" name="monsterHP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" uniqueName="monsterHP" name="monsterHP" dataDxfId="7">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterHP" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="monsterMoveSpeed" name="monsterMoveSpeed" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" uniqueName="monsterMoveSpeed" name="monsterMoveSpeed" dataDxfId="6">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterMoveSpeed" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="monsterAttackSpeed" name="monsterAttackSpeed" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" uniqueName="monsterAttackSpeed" name="monsterAttackSpeed" dataDxfId="5">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterAttackSpeed" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="monsterAttackRange" name="monsterAttackRange" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" uniqueName="monsterAttackRange" name="monsterAttackRange" dataDxfId="4">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterAttackRange" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="monsterAttack" name="monsterAttack" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" uniqueName="monsterAttack" name="monsterAttack" dataDxfId="3">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterAttack" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="monsterDefense" name="monsterDefense" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" uniqueName="monsterDefense" name="monsterDefense" dataDxfId="2">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterDefense" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="monsterPopChance" name="monsterPopChance" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" uniqueName="monsterPopChance" name="monsterPopChance" dataDxfId="1">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterPopChance" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="monsterWeight" name="monsterWeight" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" uniqueName="monsterWeight" name="monsterWeight" dataDxfId="0">
       <xmlColumnPr mapId="8" xpath="/MonsterDataBase/Field/@monsterWeight" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -1729,31 +1751,34 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="표3" displayName="표3" ref="A1:H17" tableType="xml" totalsRowShown="0" connectionId="8">
-  <autoFilter ref="A1:H17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="표3" displayName="표3" ref="A1:H22" tableType="xml" totalsRowShown="0" connectionId="8">
+  <autoFilter ref="A1:H22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
+    <sortCondition descending="1" ref="A1:A22"/>
+  </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" uniqueName="attackType" name="attackType">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" uniqueName="attackType" name="attackType">
       <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackType" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="attackXPoint" name="attackXPoint">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" uniqueName="attackXPoint" name="attackXPoint">
       <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackXPoint" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="attackYPoint" name="attackYPoint">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" uniqueName="attackYPoint" name="attackYPoint">
       <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackYPoint" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="attackXRange" name="attackXRange">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" uniqueName="attackXRange" name="attackXRange">
       <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackXRange" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="attackYRange" name="attackYRange">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" uniqueName="attackYRange" name="attackYRange">
       <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackYRange" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="attackMultiply" name="attackMultiply">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" uniqueName="attackMultiply" name="attackMultiply">
       <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@attackMultiply" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="distanceMultiply" name="distanceMultiply">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" uniqueName="distanceMultiply" name="distanceMultiply">
       <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@distanceMultiply" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="knockBack" name="knockBack">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" uniqueName="knockBack" name="knockBack">
       <xmlColumnPr mapId="12" xpath="/PlayerAttackDataBase/Field/@knockBack" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2023,7 +2048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2793,7 +2818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2947,7 +2972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3331,16 +3356,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
@@ -3377,37 +3402,37 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2">
         <v>0.8</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>172</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.5</v>
+      </c>
+      <c r="F2">
+        <v>1.5</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B3">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -3416,16 +3441,16 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="F3">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="G3">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3456,7 +3481,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B5">
         <v>0.8</v>
@@ -3468,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F5">
         <v>1.2</v>
@@ -3508,14 +3533,14 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7">
+        <v>0.8</v>
+      </c>
+      <c r="C7">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>-0.6</v>
-      </c>
       <c r="D7">
         <v>1</v>
       </c>
@@ -3523,189 +3548,189 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="G7">
+        <v>1.25</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C8" s="2">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1.2</v>
-      </c>
-      <c r="F8">
-        <v>0.5</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
+      <c r="D8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B9">
-        <v>0.8</v>
+        <v>-0.25</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="B10">
-        <v>1.2</v>
+        <v>-0.5</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="E10">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="B11">
-        <v>1.2</v>
+        <v>-0.25</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B12">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="C12">
+        <v>-0.6</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
         <v>0</v>
       </c>
-      <c r="D12">
-        <v>1.2</v>
-      </c>
-      <c r="E12">
-        <v>1.2</v>
-      </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <v>-1.25</v>
-      </c>
       <c r="H12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="B13">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="C13">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>2</v>
-      </c>
-      <c r="G13">
-        <v>1.25</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="B14">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="C14">
-        <v>-0.6</v>
+        <v>-0.4</v>
       </c>
       <c r="D14">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3716,33 +3741,33 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B15">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -3768,28 +3793,158 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
+        <v>1.2</v>
+      </c>
+      <c r="E17">
+        <v>1.2</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>-1.25</v>
+      </c>
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18">
+        <v>1.2</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1.2</v>
+      </c>
+      <c r="E18">
+        <v>1.2</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19">
+        <v>1.2</v>
+      </c>
+      <c r="C19">
+        <v>-0.6</v>
+      </c>
+      <c r="D19">
+        <v>1.2</v>
+      </c>
+      <c r="E19">
+        <v>1.2</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20">
+        <v>1.2</v>
+      </c>
+      <c r="C20">
+        <v>-0.1</v>
+      </c>
+      <c r="D20">
+        <v>1.2</v>
+      </c>
+      <c r="E20">
+        <v>0.8</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>1.25</v>
+      </c>
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="G17">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21">
+        <v>1.2</v>
+      </c>
+      <c r="C21">
         <v>0</v>
       </c>
-      <c r="H17">
-        <v>5</v>
+      <c r="D21">
+        <v>1.2</v>
+      </c>
+      <c r="E21">
+        <v>1.2</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22">
+        <v>1.2</v>
+      </c>
+      <c r="C22">
+        <v>-0.6</v>
+      </c>
+      <c r="D22">
+        <v>1.2</v>
+      </c>
+      <c r="E22">
+        <v>1.2</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
status info, repeat dialog
update
</commit_message>
<xml_diff>
--- a/Assets/Resources/XML/Database.xlsx
+++ b/Assets/Resources/XML/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="1155" windowWidth="22110" windowHeight="15435" activeTab="2"/>
+    <workbookView xWindow="1110" yWindow="1155" windowWidth="22110" windowHeight="15435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item Data" sheetId="1" r:id="rId1"/>
@@ -622,11 +622,14 @@
   <connection id="15" name="SkillDataBaseBasic2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\유니티 작업\SkillDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="16" name="SkillDataBaseBasic3" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\유니티 작업\SkillDataBaseBasic.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="228">
   <si>
     <t>itemName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1477,6 +1480,46 @@
   </si>
   <si>
     <t>뭐야?:귀찮아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillMaxStack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1843,7 +1886,24 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema7">
+  <Schema ID="Schema6">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="NPCDialogDatabase">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Field" form="unqualified">
+              <xsd:complexType>
+                <xsd:attribute name="NPCCode" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="Progress" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="Dialog" form="unqualified" type="xsd:string"/>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema8">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="SkillDataBase">
         <xsd:complexType>
@@ -1859,23 +1919,7 @@
                 <xsd:attribute name="skillDescription" form="unqualified" type="xsd:string"/>
                 <xsd:attribute name="skillOnCount" form="unqualified" type="xsd:string"/>
                 <xsd:attribute name="skillTimeDuration" form="unqualified" type="xsd:string"/>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Schema ID="Schema6">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="NPCDialogDatabase">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Field" form="unqualified">
-              <xsd:complexType>
-                <xsd:attribute name="NPCCode" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="Progress" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="Dialog" form="unqualified" type="xsd:string"/>
+                <xsd:attribute name="skillMaxStack" form="unqualified" type="xsd:string"/>
               </xsd:complexType>
             </xsd:element>
           </xsd:sequence>
@@ -1895,8 +1939,8 @@
   <Map ID="17" Name="PlayerAttackDataBase_맵" RootElement="PlayerAttackDataBase" SchemaID="Schema5" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="11" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="20" Name="SkillDataBase_맵" RootElement="SkillDataBase" SchemaID="Schema7" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="15" DataBindingLoadMode="1"/>
+  <Map ID="24" Name="SkillDataBase_맵" RootElement="SkillDataBase" SchemaID="Schema8" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="16" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
@@ -1935,32 +1979,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A1:H15" tableType="xml" totalsRowShown="0" connectionId="15">
-  <autoFilter ref="A1:H15"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A1:I15" tableType="xml" totalsRowShown="0" connectionId="16">
+  <autoFilter ref="A1:I15"/>
+  <tableColumns count="9">
     <tableColumn id="1" uniqueName="skillType" name="skillType">
-      <xmlColumnPr mapId="20" xpath="/SkillDataBase/Field/@skillType" xmlDataType="string"/>
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="skillName" name="skillName">
-      <xmlColumnPr mapId="20" xpath="/SkillDataBase/Field/@skillName" xmlDataType="string"/>
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillName" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="skillCode" name="skillCode" dataDxfId="12">
-      <xmlColumnPr mapId="20" xpath="/SkillDataBase/Field/@skillCode" xmlDataType="string"/>
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillCode" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="skillMultiply" name="skillMultiply" dataDxfId="11">
-      <xmlColumnPr mapId="20" xpath="/SkillDataBase/Field/@skillMultiply" xmlDataType="string"/>
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillMultiply" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="skillValue" name="skillValue">
-      <xmlColumnPr mapId="20" xpath="/SkillDataBase/Field/@skillValue" xmlDataType="string"/>
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillValue" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="skillDescription" name="skillDescription">
-      <xmlColumnPr mapId="20" xpath="/SkillDataBase/Field/@skillDescription" xmlDataType="string"/>
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillDescription" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="8" uniqueName="skillOnCount" name="skillOnCount" dataDxfId="10">
-      <xmlColumnPr mapId="20" xpath="/SkillDataBase/Field/@skillOnCount" xmlDataType="string"/>
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillOnCount" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="9" uniqueName="skillTimeDuration" name="skillTimeDuration">
-      <xmlColumnPr mapId="20" xpath="/SkillDataBase/Field/@skillTimeDuration" xmlDataType="string"/>
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillTimeDuration" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" uniqueName="skillMaxStack" name="skillMaxStack">
+      <xmlColumnPr mapId="24" xpath="/SkillDataBase/Field/@skillMaxStack" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3096,10 +3143,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3112,9 +3159,10 @@
     <col min="6" max="6" width="59.125" customWidth="1"/>
     <col min="7" max="7" width="15.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.375" customWidth="1"/>
+    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3139,8 +3187,11 @@
       <c r="H1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>201</v>
       </c>
@@ -3165,8 +3216,11 @@
       <c r="H2" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>202</v>
       </c>
@@ -3191,8 +3245,11 @@
       <c r="H3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>203</v>
       </c>
@@ -3217,8 +3274,11 @@
       <c r="H4" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>201</v>
       </c>
@@ -3243,8 +3303,11 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>201</v>
       </c>
@@ -3269,8 +3332,11 @@
       <c r="H6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>204</v>
       </c>
@@ -3295,8 +3361,11 @@
       <c r="H7" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>205</v>
       </c>
@@ -3321,8 +3390,11 @@
       <c r="H8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>206</v>
       </c>
@@ -3347,8 +3419,11 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>201</v>
       </c>
@@ -3373,8 +3448,11 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>208</v>
       </c>
@@ -3399,8 +3477,11 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>208</v>
       </c>
@@ -3425,8 +3506,11 @@
       <c r="H12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>208</v>
       </c>
@@ -3451,8 +3535,11 @@
       <c r="H13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>209</v>
       </c>
@@ -3477,8 +3564,11 @@
       <c r="H14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>208</v>
       </c>
@@ -3502,6 +3592,9 @@
       </c>
       <c r="H15" s="1">
         <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3519,7 +3612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
save delete, enchant skill
update
</commit_message>
<xml_diff>
--- a/Assets/Resources/XML/Database.xlsx
+++ b/Assets/Resources/XML/Database.xlsx
@@ -648,7 +648,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="432">
   <si>
     <t>itemName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1610,733 +1610,749 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>왔구나? 항상 있는 일이지만 매번 손이 부족해..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래, 창 다루는건 많이 익숙해 졌나?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실력도 확인해 볼 겸, 같이갈테냐?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좋아, 준비됐으면 가볼까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Answer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Answer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래? 그럼 좀 부탁해볼까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScrollAllTown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TutorialSelect</t>
+  </si>
+  <si>
+    <t>TutorialBattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이번엔 제법 몰려왔네.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격 하는 법은 잊지 않았겠지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X 키를 눌러서 공격이 가능해.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앞으로 가면서나 위를 보면서 공격해도 연계 공격이 나가지.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여러 번 눌러서 연계할 수 있고,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점프한 채로 연속 공격하면 점프 연계기가 나가고,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Space bar 를 누르면 회피할 수 있을거야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여긴 맡기고 가마. 나는 다른곳으로 가볼테니.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네, 조심하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstBattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조금 많아보이는데...?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정신차리고 해보자!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetBell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항상 도움만 받네요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘도 고생하셨어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래도 오늘은 얘가 도와줘서 수고를 덜었어.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이제 무기도 잘 다루는 것 같고 탑에 가도 되겠는데?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>와! 정말로 가도 되나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>축하드려요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항상 기대하고 계셨잖아요!</t>
+  </si>
+  <si>
+    <t>Enchanter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enchanter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아, 참!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠시만 기다려주세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탑에 갈 수 있는 허락도 받으셨고,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이걸 드릴게요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첫 실전도 아무 탈 없이 해낸 기념으로…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고마워! 이건 종이야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부적이라나봐요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나쁜 일을 막아준다는 얘기가 있어요. 많이 비싼거에요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제로 몬스터의 공격은 막아주진 못하겠지만요…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래도 고마워.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘 가지고 다닐게!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enchanter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Camera</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>그럼 저, 이제 가봐도 될까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>준비는 철저히 하고, 조심해서 다녀오도록 해라.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네, 당연하죠!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아, 그리고 이걸 들고가거라.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이게 뭐에요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탑에 들어갈 수 있는 열쇠.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탑 입구에 집어넣으면 문이 열릴거야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키가 부족해지면 주변의 몬스터를 잡아서 얻을 수 있지.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감사합니다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다녀올게요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래, 탑에 갔다 돌아오지 못한 사람은 없지만,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TutorialBattle/GameObject/Event_Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstTalkShop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>CameraFocus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Merchant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merchant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안녕하세요! 오늘은 물건이 들어왔나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아니, 타워에도 안들어간지 오래됐고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도시에서는 물자에관한 연락도 없어.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>며칠째 이러고 있는지 모르겠네.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일단 남은건 있는데 보고갈래?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐? 드디어 허가가 나온거냐?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네! 혹시, 탑 열쇠는 있나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네, 허락은 받았어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이제 탑에 갈려고하는데 열쇠가 없어서요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈은 별로 없지만요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기껏해야 도시에 관상용으로 팔릴뿐이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혹시, 남는게 있으면 나한테 팔아.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어짜피 열쇠는 다른데에 쓰지도 못해.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도시에 가서 팔아야겠다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merchant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merchant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstTalkEnchanter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실험하고 있는건 잘 되어가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아뇨, 아직 진전이 없어요…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 열쇠를 잘 활용하면 장비에도 사용할 수 있을거 같은데…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도움이 필요한 일이 있으면 말해줘, 도와줄게.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감사합니다. 뭔가 생각 나는게 있으면 말씀드릴게요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스승님, 제가 탑에 갈 수 있게 해주셔서 감사합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허허, 내가 준비가 됐다고는 했지만, 부족한 부분이 있다고 생각되면 다시 나를 찾아와.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헤헤, 넵. 아직 부족하다 생각되면 말씀드릴게요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낮 시간대는 힘들고, 저녁에 찾아오면 훈련시켜주마.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enchanter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enchanter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enchanter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Trainer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstTalkTrainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstEnterTower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탑 입구에 열쇠를 넣으라고 했었지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>와… 좋아, 가보자!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstInTower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>응? 눈 깜작할 새에 하늘로 올라왔어…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그럼 조심해서 가볼까.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstDead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>으윽…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstDead/GameObject/???</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…후우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstRecall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헉…!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…? 분명히 탑에서 쓰러졌는데… 꿈이었나?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstBoss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss_Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstBoss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스승님…? 왜 여기 계세요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수색하러 가신게 아닌가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss_Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss_Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PlayerCharacter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>왔구나? 항상 있는 일이지만 매번 손이 부족해..</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래, 창 다루는건 많이 익숙해 졌나?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>실력도 확인해 볼 겸, 같이갈테냐?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Select</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>좋아, 준비됐으면 가볼까?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Answer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Answer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래? 그럼 좀 부탁해볼까?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScrollAllTown</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TutorialSelect</t>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraFocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(트레이너 준비모션)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(타워 스크롤)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(카메라 진동 및 문 애니매이션?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(열쇠 이미지 띄우기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(벨 이미지 띄우기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마을 스크롤)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstBossEnd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…스승님?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…아직 탑에오는건 이르다고 생각했는데…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강하구나…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스승님이 허락해 주셨잖아요…!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그런가…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(트레이너가 쓰러지고 사라지는 모션)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss_Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss_Trainer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPCCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EventNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네, 도와드릴게요. 잘부탁드립니다.:5:TutorialSelect:1@충분히 익숙해졌어요. 제가 맡겠습니다.:6:TutorialSelect:2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraScroll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start:End:0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstBattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tower_Forest_Start:Tower_Forest_End:0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Town_Start:Town_End:0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TutorialBattle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이번엔 제법 몰려왔네.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격 하는 법은 잊지 않았겠지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X 키를 눌러서 공격이 가능해.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>앞으로 가면서나 위를 보면서 공격해도 연계 공격이 나가지.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여러 번 눌러서 연계할 수 있고,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>점프한 채로 연속 공격하면 점프 연계기가 나가고,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Space bar 를 누르면 회피할 수 있을거야.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여긴 맡기고 가마. 나는 다른곳으로 가볼테니.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네, 조심하세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstBattle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조금 많아보이는데...?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정신차리고 해보자!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetBell</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>항상 도움만 받네요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘도 고생하셨어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래도 오늘은 얘가 도와줘서 수고를 덜었어.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이제 무기도 잘 다루는 것 같고 탑에 가도 되겠는데?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>와! 정말로 가도 되나요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>축하드려요!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>항상 기대하고 계셨잖아요!</t>
-  </si>
-  <si>
-    <t>Enchanter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enchanter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아, 참!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잠시만 기다려주세요!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탑에 갈 수 있는 허락도 받으셨고,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이걸 드릴게요!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>첫 실전도 아무 탈 없이 해낸 기념으로…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고마워! 이건 종이야?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부적이라나봐요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나쁜 일을 막아준다는 얘기가 있어요. 많이 비싼거에요!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>실제로 몬스터의 공격은 막아주진 못하겠지만요…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래도 고마워.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잘 가지고 다닐게!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enchanter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Camera</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그럼 저, 이제 가봐도 될까요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>준비는 철저히 하고, 조심해서 다녀오도록 해라.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네, 당연하죠!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아, 그리고 이걸 들고가거라.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Camera</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이게 뭐에요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탑에 들어갈 수 있는 열쇠.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탑 입구에 집어넣으면 문이 열릴거야.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>키가 부족해지면 주변의 몬스터를 잡아서 얻을 수 있지.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감사합니다!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다녀올게요!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래, 탑에 갔다 돌아오지 못한 사람은 없지만,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TutorialBattle/GameObject/Event_Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstTalkShop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Merchant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Merchant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안녕하세요! 오늘은 물건이 들어왔나요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아니, 타워에도 안들어간지 오래됐고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도시에서는 물자에관한 연락도 없어.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>며칠째 이러고 있는지 모르겠네.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일단 남은건 있는데 보고갈래?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뭐? 드디어 허가가 나온거냐?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네! 혹시, 탑 열쇠는 있나요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네, 허락은 받았어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이제 탑에 갈려고하는데 열쇠가 없어서요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돈은 별로 없지만요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기껏해야 도시에 관상용으로 팔릴뿐이다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>혹시, 남는게 있으면 나한테 팔아.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>어짜피 열쇠는 다른데에 쓰지도 못해.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도시에 가서 팔아야겠다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Merchant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Merchant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstTalkEnchanter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>실험하고 있는건 잘 되어가?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아뇨, 아직 진전이 없어요…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 열쇠를 잘 활용하면 장비에도 사용할 수 있을거 같은데…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도움이 필요한 일이 있으면 말해줘, 도와줄게.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감사합니다. 뭔가 생각 나는게 있으면 말씀드릴게요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스승님, 제가 탑에 갈 수 있게 해주셔서 감사합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>허허, 내가 준비가 됐다고는 했지만, 부족한 부분이 있다고 생각되면 다시 나를 찾아와.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>헤헤, 넵. 아직 부족하다 생각되면 말씀드릴게요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>낮 시간대는 힘들고, 저녁에 찾아오면 훈련시켜주마.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enchanter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enchanter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enchanter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstTalkTrainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstEnterTower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탑 입구에 열쇠를 넣으라고 했었지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Camera</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>와… 좋아, 가보자!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstInTower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>응? 눈 깜작할 새에 하늘로 올라왔어…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그럼 조심해서 가볼까.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstDead</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>으윽…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Camera</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstDead/GameObject/???</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…후우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstRecall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>헉…!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…? 분명히 탑에서 쓰러졌는데… 꿈이었나?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstBoss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss_Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstBoss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스승님…? 왜 여기 계세요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수색하러 가신게 아닌가?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Camera</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…!!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss_Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss_Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerCharacter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CameraFocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(트레이너 준비모션)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(타워 스크롤)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(카메라 진동 및 문 애니매이션?)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(열쇠 이미지 띄우기)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(벨 이미지 띄우기)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마을 스크롤)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstBossEnd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…스승님?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…아직 탑에오는건 이르다고 생각했는데…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강하구나…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스승님이 허락해 주셨잖아요…!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그런가…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(트레이너가 쓰러지고 사라지는 모션)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss_Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss_Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPCCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EventNumber</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네, 도와드릴게요. 잘부탁드립니다.:5:TutorialSelect:1@충분히 익숙해졌어요. 제가 맡겠습니다.:6:TutorialSelect:2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CameraScroll</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Start:End</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Camera</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2971,8 +2987,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="표6" displayName="표6" ref="A1:F104" tableType="xml" totalsRowShown="0" connectionId="3">
-  <autoFilter ref="A1:F104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="표6" displayName="표6" ref="A1:F106" tableType="xml" totalsRowShown="0" connectionId="3">
+  <autoFilter ref="A1:F106"/>
   <tableColumns count="6">
     <tableColumn id="1" uniqueName="EventName" name="EventName" dataDxfId="5">
       <xmlColumnPr mapId="28" xpath="/EventListDataBase/EventList/EventName" xmlDataType="string"/>
@@ -5630,10 +5646,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5679,7 +5695,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>238</v>
@@ -5748,7 +5764,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -5757,16 +5773,18 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>423</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -5775,18 +5793,18 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>247</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
@@ -5799,12 +5817,12 @@
         <v>94</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
@@ -5814,69 +5832,69 @@
         <v>230</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>261</v>
+        <v>430</v>
       </c>
       <c r="B13" s="2">
         <v>3</v>
@@ -5885,36 +5903,34 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>262</v>
+        <v>431</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>264</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>228</v>
+        <v>261</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2">
@@ -5924,15 +5940,15 @@
         <v>228</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2">
@@ -5942,15 +5958,15 @@
         <v>228</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
@@ -5960,7 +5976,7 @@
         <v>228</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>267</v>
@@ -5968,7 +5984,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2">
@@ -5978,15 +5994,15 @@
         <v>228</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2">
@@ -5996,15 +6012,15 @@
         <v>228</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2">
@@ -6014,15 +6030,15 @@
         <v>228</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2">
@@ -6032,873 +6048,871 @@
         <v>228</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>272</v>
+        <v>320</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B22" s="2">
-        <v>3</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>275</v>
+        <v>228</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>427</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3</v>
+      </c>
       <c r="C23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>228</v>
+        <v>423</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>277</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B24" s="2">
-        <v>4</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="B24" s="2"/>
       <c r="C24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>287</v>
+        <v>247</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>303</v>
+        <v>228</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B26" s="2"/>
+        <v>277</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4</v>
+      </c>
       <c r="C26" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>303</v>
+        <v>245</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>248</v>
+        <v>282</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>288</v>
+        <v>247</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E38" s="1"/>
+        <v>302</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="F38" s="1" t="s">
-        <v>405</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>287</v>
-      </c>
+      <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>297</v>
+        <v>404</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>248</v>
+        <v>287</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>248</v>
+        <v>301</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>228</v>
+        <v>302</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>316</v>
+        <v>247</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>228</v>
+        <v>302</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>317</v>
+        <v>247</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>248</v>
+        <v>316</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>94</v>
+        <v>318</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E50" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="F50" s="1" t="s">
-        <v>404</v>
+        <v>306</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>248</v>
+        <v>94</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>319</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
-        <v>311</v>
+        <v>403</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>94</v>
+        <v>247</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>248</v>
+        <v>94</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B57" s="2">
-        <v>5</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="B57" s="2"/>
       <c r="C57" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>323</v>
+        <v>228</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>322</v>
+        <v>277</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>325</v>
+        <v>228</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B59" s="2">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2">
-        <v>3</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>324</v>
+        <v>247</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>248</v>
+        <v>323</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>343</v>
+        <v>247</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>338</v>
@@ -6906,371 +6920,369 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B71" s="2">
-        <v>5</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="B71" s="2"/>
       <c r="C71" s="2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>246</v>
+        <v>345</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>228</v>
+        <v>345</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B73" s="2">
+        <v>5</v>
+      </c>
+      <c r="C73" s="2">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2">
-        <v>3</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>360</v>
-      </c>
       <c r="F73" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>345</v>
+        <v>228</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="B77" s="2">
+        <v>346</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2">
         <v>5</v>
       </c>
-      <c r="C77" s="2">
-        <v>1</v>
-      </c>
       <c r="D77" s="1" t="s">
-        <v>246</v>
+        <v>344</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="B79" s="2"/>
+        <v>364</v>
+      </c>
+      <c r="B79" s="2">
+        <v>5</v>
+      </c>
       <c r="C79" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>345</v>
+        <v>245</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>345</v>
+        <v>228</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B81" s="2">
-        <v>5</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="B81" s="2"/>
       <c r="C81" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>246</v>
+        <v>344</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>248</v>
+        <v>363</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="E82" s="1"/>
+        <v>344</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="F82" s="1" t="s">
-        <v>403</v>
+        <v>356</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B83" s="2"/>
+        <v>365</v>
+      </c>
+      <c r="B83" s="2">
+        <v>5</v>
+      </c>
       <c r="C83" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>426</v>
+        <v>368</v>
       </c>
       <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B85" s="2">
-        <v>6</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="B85" s="2"/>
       <c r="C85" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>373</v>
+        <v>228</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>402</v>
-      </c>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B87" s="2">
+        <v>6</v>
+      </c>
+      <c r="C87" s="2">
+        <v>1</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2">
-        <v>3</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>375</v>
-      </c>
       <c r="E87" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B88" s="2">
-        <v>7</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="B88" s="2"/>
       <c r="C88" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>246</v>
+        <v>423</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>348</v>
+        <v>426</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>378</v>
+        <v>401</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>246</v>
+        <v>374</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>380</v>
+        <v>247</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B90" s="2">
         <v>7</v>
@@ -7279,36 +7291,36 @@
         <v>1</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>248</v>
+        <v>347</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2">
         <v>2</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>348</v>
+        <v>379</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B92" s="2">
         <v>7</v>
@@ -7317,227 +7329,265 @@
         <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>386</v>
+        <v>245</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>387</v>
+        <v>247</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2">
         <v>2</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>248</v>
+        <v>347</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="B94" s="2"/>
+        <v>384</v>
+      </c>
+      <c r="B94" s="2">
+        <v>7</v>
+      </c>
       <c r="C94" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>367</v>
+        <v>245</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>398</v>
+        <v>247</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>375</v>
+        <v>398</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="E97" s="1"/>
+        <v>366</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F97" s="1" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>400</v>
+        <v>374</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B99" s="2">
-        <v>8</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="B99" s="2"/>
       <c r="C99" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>248</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>228</v>
+        <v>399</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B101" s="2">
+        <v>8</v>
+      </c>
+      <c r="C101" s="2">
+        <v>1</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2">
-        <v>3</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>228</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>248</v>
+        <v>386</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2">
+        <v>4</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2">
+        <v>5</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2">
         <v>6</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1" t="s">
-        <v>415</v>
+      <c r="D106" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -7568,10 +7618,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" t="s">
         <v>418</v>
-      </c>
-      <c r="B1" t="s">
-        <v>419</v>
       </c>
       <c r="C1" t="s">
         <v>226</v>
@@ -7585,10 +7635,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>37</v>
@@ -7599,7 +7649,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>37</v>

</xml_diff>